<commit_message>
updated with nb date
</commit_message>
<xml_diff>
--- a/Data/PPI_samlet_DK.xlsx
+++ b/Data/PPI_samlet_DK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjhp/Desktop/Inflation-Forecast/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3365E899-6A4F-874B-9954-F02A70D755C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11501511-159D-C441-9344-8732065D2DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="282">
   <si>
     <t>2005M01</t>
   </si>
@@ -753,12 +753,126 @@
   <si>
     <t>date</t>
   </si>
+  <si>
+    <t>BCDE Råstofindvinding, Industri, Energi- og Vandforsyning</t>
+  </si>
+  <si>
+    <t>BC Råstofindvinding og industri</t>
+  </si>
+  <si>
+    <t>B Råstofindvinding</t>
+  </si>
+  <si>
+    <t>C Fremstillingsvirksomhed</t>
+  </si>
+  <si>
+    <t>10 Fremstilling af fødevarer</t>
+  </si>
+  <si>
+    <t>101 Forarbejdning og konservering af kød og produktion af kødprodukter</t>
+  </si>
+  <si>
+    <t>102 Forarbejdning og konservering af fisk, krebsdyr og bløddyr</t>
+  </si>
+  <si>
+    <t>105 Fremstilling af mejeriprodukter</t>
+  </si>
+  <si>
+    <t>107 Fremstilling af bageri- og dejprodukter</t>
+  </si>
+  <si>
+    <t>108 Fremstilling af andre fødevarer</t>
+  </si>
+  <si>
+    <t>11 Fremstilling af drikkevarer</t>
+  </si>
+  <si>
+    <t>12 Fremstilling af tobaksprodukter</t>
+  </si>
+  <si>
+    <t>13 Fremstilling af tekstiler</t>
+  </si>
+  <si>
+    <t>14 Fremstilling af beklædningsartikler</t>
+  </si>
+  <si>
+    <t>15 Fremstilling af læder og lædervarer</t>
+  </si>
+  <si>
+    <t>16 Fremstilling af træ og varer af træ og kork, undtagen møbler; fremstilling af varer af strå og flettematerialer</t>
+  </si>
+  <si>
+    <t>17 Fremstilling af papir og papirvarer</t>
+  </si>
+  <si>
+    <t>18 Trykning og reproduktion af indspillede medier</t>
+  </si>
+  <si>
+    <t>21 Fremstilling af farmaceutiske råvarer og farmaceutiske præparater</t>
+  </si>
+  <si>
+    <t>22 Fremstilling af gummi- og plastprodukter</t>
+  </si>
+  <si>
+    <t>23 Fremstilling af andre ikke-metalholdige mineralske produkter</t>
+  </si>
+  <si>
+    <t>24 Fremstilling af metal</t>
+  </si>
+  <si>
+    <t>25 Jern- og metalvareindustri, undtagen maskiner og udstyr</t>
+  </si>
+  <si>
+    <t>26 Fremstilling af computere, elektroniske og optiske produkter</t>
+  </si>
+  <si>
+    <t>27 Fremstilling af elektrisk udstyr</t>
+  </si>
+  <si>
+    <t>28 Fremstilling af maskiner og udstyr i.a.n.</t>
+  </si>
+  <si>
+    <t>29 Fremstilling af motorkøretøjer, påhængsvogne og sættevogne</t>
+  </si>
+  <si>
+    <t>30 Fremstilling af andre transportmidler</t>
+  </si>
+  <si>
+    <t>31 Fremstilling af møbler</t>
+  </si>
+  <si>
+    <t>32 Anden fremstillingsvirksomhed</t>
+  </si>
+  <si>
+    <t>D El-, gas- og fjernvarmeforsyning</t>
+  </si>
+  <si>
+    <t>S1 Investeringsgodeindustri</t>
+  </si>
+  <si>
+    <t>S2 Mellemproduktindustri</t>
+  </si>
+  <si>
+    <t>S3 Fremstilling af varige forbrugsgoder</t>
+  </si>
+  <si>
+    <t>S4 Fremstilling af ikke-varige forbrugsgoder</t>
+  </si>
+  <si>
+    <t>S5 Fremstilling af energiprodukter og energiforsyning</t>
+  </si>
+  <si>
+    <t>C33 Fremstillingsindustri ekskl. forarb. af kød og fisk samt ekskl. fremst. af tobak, koks og raffinerede mineral olieprodukter</t>
+  </si>
+  <si>
+    <t>S6 Fremstilling af forbrugsgoder ekskl. fødevarer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1114,57 +1228,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC94715-C267-3241-9CB0-694716E167F9}">
   <dimension ref="A1:AN244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="25" workbookViewId="0">
-      <selection activeCell="H258" sqref="H258"/>
+    <sheetView tabSelected="1" zoomScale="36" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AM1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="AN1" s="1"/>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1398,7 @@
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1322,7 +1512,7 @@
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1436,7 +1626,7 @@
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1740,7 @@
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1664,7 +1854,7 @@
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1778,7 +1968,7 @@
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1892,7 +2082,7 @@
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2006,7 +2196,7 @@
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2120,7 +2310,7 @@
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2234,7 +2424,7 @@
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2348,7 +2538,7 @@
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2462,7 +2652,7 @@
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2576,7 +2766,7 @@
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2690,7 +2880,7 @@
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2804,7 +2994,7 @@
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2918,7 +3108,7 @@
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -3032,7 +3222,7 @@
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -3146,7 +3336,7 @@
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -3260,7 +3450,7 @@
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -3374,7 +3564,7 @@
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
     </row>
-    <row r="22" spans="1:40">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -3488,7 +3678,7 @@
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
     </row>
-    <row r="23" spans="1:40">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3602,7 +3792,7 @@
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
     </row>
-    <row r="24" spans="1:40">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -3716,7 +3906,7 @@
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
     </row>
-    <row r="25" spans="1:40">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3830,7 +4020,7 @@
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
     </row>
-    <row r="26" spans="1:40">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -3944,7 +4134,7 @@
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
     </row>
-    <row r="27" spans="1:40">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -4058,7 +4248,7 @@
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
     </row>
-    <row r="28" spans="1:40">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -4172,7 +4362,7 @@
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
     </row>
-    <row r="29" spans="1:40">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -4286,7 +4476,7 @@
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
     </row>
-    <row r="30" spans="1:40">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -4400,7 +4590,7 @@
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
     </row>
-    <row r="31" spans="1:40">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -4514,7 +4704,7 @@
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
     </row>
-    <row r="32" spans="1:40">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -4628,7 +4818,7 @@
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -4742,7 +4932,7 @@
       <c r="AM33" s="2"/>
       <c r="AN33" s="2"/>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -4856,7 +5046,7 @@
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -4970,7 +5160,7 @@
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -5084,7 +5274,7 @@
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
     </row>
-    <row r="37" spans="1:40">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -5198,7 +5388,7 @@
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -5312,7 +5502,7 @@
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -5426,7 +5616,7 @@
       <c r="AM39" s="2"/>
       <c r="AN39" s="2"/>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -5540,7 +5730,7 @@
       <c r="AM40" s="2"/>
       <c r="AN40" s="2"/>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -5654,7 +5844,7 @@
       <c r="AM41" s="2"/>
       <c r="AN41" s="2"/>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -5768,7 +5958,7 @@
       <c r="AM42" s="2"/>
       <c r="AN42" s="2"/>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -5882,7 +6072,7 @@
       <c r="AM43" s="2"/>
       <c r="AN43" s="2"/>
     </row>
-    <row r="44" spans="1:40">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -5996,7 +6186,7 @@
       <c r="AM44" s="2"/>
       <c r="AN44" s="2"/>
     </row>
-    <row r="45" spans="1:40">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -6110,7 +6300,7 @@
       <c r="AM45" s="2"/>
       <c r="AN45" s="2"/>
     </row>
-    <row r="46" spans="1:40">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -6224,7 +6414,7 @@
       <c r="AM46" s="2"/>
       <c r="AN46" s="2"/>
     </row>
-    <row r="47" spans="1:40">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -6338,7 +6528,7 @@
       <c r="AM47" s="2"/>
       <c r="AN47" s="2"/>
     </row>
-    <row r="48" spans="1:40">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -6452,7 +6642,7 @@
       <c r="AM48" s="2"/>
       <c r="AN48" s="2"/>
     </row>
-    <row r="49" spans="1:40">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -6566,7 +6756,7 @@
       <c r="AM49" s="2"/>
       <c r="AN49" s="2"/>
     </row>
-    <row r="50" spans="1:40">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -6680,7 +6870,7 @@
       <c r="AM50" s="2"/>
       <c r="AN50" s="2"/>
     </row>
-    <row r="51" spans="1:40">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -6794,7 +6984,7 @@
       <c r="AM51" s="2"/>
       <c r="AN51" s="2"/>
     </row>
-    <row r="52" spans="1:40">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -6908,7 +7098,7 @@
       <c r="AM52" s="2"/>
       <c r="AN52" s="2"/>
     </row>
-    <row r="53" spans="1:40">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -7022,7 +7212,7 @@
       <c r="AM53" s="2"/>
       <c r="AN53" s="2"/>
     </row>
-    <row r="54" spans="1:40">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -7136,7 +7326,7 @@
       <c r="AM54" s="2"/>
       <c r="AN54" s="2"/>
     </row>
-    <row r="55" spans="1:40">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -7250,7 +7440,7 @@
       <c r="AM55" s="2"/>
       <c r="AN55" s="2"/>
     </row>
-    <row r="56" spans="1:40">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -7364,7 +7554,7 @@
       <c r="AM56" s="2"/>
       <c r="AN56" s="2"/>
     </row>
-    <row r="57" spans="1:40">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -7478,7 +7668,7 @@
       <c r="AM57" s="2"/>
       <c r="AN57" s="2"/>
     </row>
-    <row r="58" spans="1:40">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -7592,7 +7782,7 @@
       <c r="AM58" s="2"/>
       <c r="AN58" s="2"/>
     </row>
-    <row r="59" spans="1:40">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -7706,7 +7896,7 @@
       <c r="AM59" s="2"/>
       <c r="AN59" s="2"/>
     </row>
-    <row r="60" spans="1:40">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -7820,7 +8010,7 @@
       <c r="AM60" s="2"/>
       <c r="AN60" s="2"/>
     </row>
-    <row r="61" spans="1:40">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -7934,7 +8124,7 @@
       <c r="AM61" s="2"/>
       <c r="AN61" s="2"/>
     </row>
-    <row r="62" spans="1:40">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -8048,7 +8238,7 @@
       <c r="AM62" s="2"/>
       <c r="AN62" s="2"/>
     </row>
-    <row r="63" spans="1:40">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -8162,7 +8352,7 @@
       <c r="AM63" s="2"/>
       <c r="AN63" s="2"/>
     </row>
-    <row r="64" spans="1:40">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -8276,7 +8466,7 @@
       <c r="AM64" s="2"/>
       <c r="AN64" s="2"/>
     </row>
-    <row r="65" spans="1:40">
+    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
@@ -8390,7 +8580,7 @@
       <c r="AM65" s="2"/>
       <c r="AN65" s="2"/>
     </row>
-    <row r="66" spans="1:40">
+    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
@@ -8504,7 +8694,7 @@
       <c r="AM66" s="2"/>
       <c r="AN66" s="2"/>
     </row>
-    <row r="67" spans="1:40">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -8618,7 +8808,7 @@
       <c r="AM67" s="2"/>
       <c r="AN67" s="2"/>
     </row>
-    <row r="68" spans="1:40">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
@@ -8732,7 +8922,7 @@
       <c r="AM68" s="2"/>
       <c r="AN68" s="2"/>
     </row>
-    <row r="69" spans="1:40">
+    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -8846,7 +9036,7 @@
       <c r="AM69" s="2"/>
       <c r="AN69" s="2"/>
     </row>
-    <row r="70" spans="1:40">
+    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -8960,7 +9150,7 @@
       <c r="AM70" s="2"/>
       <c r="AN70" s="2"/>
     </row>
-    <row r="71" spans="1:40">
+    <row r="71" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
@@ -9074,7 +9264,7 @@
       <c r="AM71" s="2"/>
       <c r="AN71" s="2"/>
     </row>
-    <row r="72" spans="1:40">
+    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
@@ -9188,7 +9378,7 @@
       <c r="AM72" s="2"/>
       <c r="AN72" s="2"/>
     </row>
-    <row r="73" spans="1:40">
+    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
@@ -9302,7 +9492,7 @@
       <c r="AM73" s="2"/>
       <c r="AN73" s="2"/>
     </row>
-    <row r="74" spans="1:40">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
@@ -9416,7 +9606,7 @@
       <c r="AM74" s="2"/>
       <c r="AN74" s="2"/>
     </row>
-    <row r="75" spans="1:40">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -9530,7 +9720,7 @@
       <c r="AM75" s="2"/>
       <c r="AN75" s="2"/>
     </row>
-    <row r="76" spans="1:40">
+    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -9644,7 +9834,7 @@
       <c r="AM76" s="2"/>
       <c r="AN76" s="2"/>
     </row>
-    <row r="77" spans="1:40">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -9758,7 +9948,7 @@
       <c r="AM77" s="2"/>
       <c r="AN77" s="2"/>
     </row>
-    <row r="78" spans="1:40">
+    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -9872,7 +10062,7 @@
       <c r="AM78" s="2"/>
       <c r="AN78" s="2"/>
     </row>
-    <row r="79" spans="1:40">
+    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
@@ -9986,7 +10176,7 @@
       <c r="AM79" s="2"/>
       <c r="AN79" s="2"/>
     </row>
-    <row r="80" spans="1:40">
+    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -10100,7 +10290,7 @@
       <c r="AM80" s="2"/>
       <c r="AN80" s="2"/>
     </row>
-    <row r="81" spans="1:40">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -10214,7 +10404,7 @@
       <c r="AM81" s="2"/>
       <c r="AN81" s="2"/>
     </row>
-    <row r="82" spans="1:40">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -10328,7 +10518,7 @@
       <c r="AM82" s="2"/>
       <c r="AN82" s="2"/>
     </row>
-    <row r="83" spans="1:40">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -10442,7 +10632,7 @@
       <c r="AM83" s="2"/>
       <c r="AN83" s="2"/>
     </row>
-    <row r="84" spans="1:40">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -10556,7 +10746,7 @@
       <c r="AM84" s="2"/>
       <c r="AN84" s="2"/>
     </row>
-    <row r="85" spans="1:40">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -10670,7 +10860,7 @@
       <c r="AM85" s="2"/>
       <c r="AN85" s="2"/>
     </row>
-    <row r="86" spans="1:40">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -10784,7 +10974,7 @@
       <c r="AM86" s="2"/>
       <c r="AN86" s="2"/>
     </row>
-    <row r="87" spans="1:40">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -10898,7 +11088,7 @@
       <c r="AM87" s="2"/>
       <c r="AN87" s="2"/>
     </row>
-    <row r="88" spans="1:40">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -11012,7 +11202,7 @@
       <c r="AM88" s="2"/>
       <c r="AN88" s="2"/>
     </row>
-    <row r="89" spans="1:40">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -11126,7 +11316,7 @@
       <c r="AM89" s="2"/>
       <c r="AN89" s="2"/>
     </row>
-    <row r="90" spans="1:40">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -11240,7 +11430,7 @@
       <c r="AM90" s="2"/>
       <c r="AN90" s="2"/>
     </row>
-    <row r="91" spans="1:40">
+    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -11354,7 +11544,7 @@
       <c r="AM91" s="2"/>
       <c r="AN91" s="2"/>
     </row>
-    <row r="92" spans="1:40">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -11468,7 +11658,7 @@
       <c r="AM92" s="2"/>
       <c r="AN92" s="2"/>
     </row>
-    <row r="93" spans="1:40">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -11582,7 +11772,7 @@
       <c r="AM93" s="2"/>
       <c r="AN93" s="2"/>
     </row>
-    <row r="94" spans="1:40">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
@@ -11696,7 +11886,7 @@
       <c r="AM94" s="2"/>
       <c r="AN94" s="2"/>
     </row>
-    <row r="95" spans="1:40">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
@@ -11810,7 +12000,7 @@
       <c r="AM95" s="2"/>
       <c r="AN95" s="2"/>
     </row>
-    <row r="96" spans="1:40">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -11924,7 +12114,7 @@
       <c r="AM96" s="2"/>
       <c r="AN96" s="2"/>
     </row>
-    <row r="97" spans="1:40">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -12038,7 +12228,7 @@
       <c r="AM97" s="2"/>
       <c r="AN97" s="2"/>
     </row>
-    <row r="98" spans="1:40">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -12152,7 +12342,7 @@
       <c r="AM98" s="2"/>
       <c r="AN98" s="2"/>
     </row>
-    <row r="99" spans="1:40">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -12266,7 +12456,7 @@
       <c r="AM99" s="2"/>
       <c r="AN99" s="2"/>
     </row>
-    <row r="100" spans="1:40">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -12380,7 +12570,7 @@
       <c r="AM100" s="2"/>
       <c r="AN100" s="2"/>
     </row>
-    <row r="101" spans="1:40">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -12494,7 +12684,7 @@
       <c r="AM101" s="2"/>
       <c r="AN101" s="2"/>
     </row>
-    <row r="102" spans="1:40">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -12608,7 +12798,7 @@
       <c r="AM102" s="2"/>
       <c r="AN102" s="2"/>
     </row>
-    <row r="103" spans="1:40">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
@@ -12722,7 +12912,7 @@
       <c r="AM103" s="2"/>
       <c r="AN103" s="2"/>
     </row>
-    <row r="104" spans="1:40">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -12836,7 +13026,7 @@
       <c r="AM104" s="2"/>
       <c r="AN104" s="2"/>
     </row>
-    <row r="105" spans="1:40">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -12950,7 +13140,7 @@
       <c r="AM105" s="2"/>
       <c r="AN105" s="2"/>
     </row>
-    <row r="106" spans="1:40">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -13064,7 +13254,7 @@
       <c r="AM106" s="2"/>
       <c r="AN106" s="2"/>
     </row>
-    <row r="107" spans="1:40">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -13178,7 +13368,7 @@
       <c r="AM107" s="2"/>
       <c r="AN107" s="2"/>
     </row>
-    <row r="108" spans="1:40">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -13292,7 +13482,7 @@
       <c r="AM108" s="2"/>
       <c r="AN108" s="2"/>
     </row>
-    <row r="109" spans="1:40">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -13406,7 +13596,7 @@
       <c r="AM109" s="2"/>
       <c r="AN109" s="2"/>
     </row>
-    <row r="110" spans="1:40">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -13520,7 +13710,7 @@
       <c r="AM110" s="2"/>
       <c r="AN110" s="2"/>
     </row>
-    <row r="111" spans="1:40">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
@@ -13638,7 +13828,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="112" spans="1:40">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -13756,7 +13946,7 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="113" spans="1:40">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -13874,7 +14064,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="114" spans="1:40">
+    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -13992,7 +14182,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="115" spans="1:40">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -14110,7 +14300,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="116" spans="1:40">
+    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
@@ -14228,7 +14418,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="117" spans="1:40">
+    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -14346,7 +14536,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:40">
+    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -14464,7 +14654,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:40">
+    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -14582,7 +14772,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="120" spans="1:40">
+    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
@@ -14700,7 +14890,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="121" spans="1:40">
+    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
@@ -14818,7 +15008,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="122" spans="1:40">
+    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
@@ -14936,7 +15126,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="123" spans="1:40">
+    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
@@ -15054,7 +15244,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="124" spans="1:40">
+    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
@@ -15172,7 +15362,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="125" spans="1:40">
+    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
@@ -15290,7 +15480,7 @@
         <v>-14.3</v>
       </c>
     </row>
-    <row r="126" spans="1:40">
+    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
@@ -15408,7 +15598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:40">
+    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
@@ -15526,7 +15716,7 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="128" spans="1:40">
+    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -15644,7 +15834,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="129" spans="1:40">
+    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
@@ -15762,7 +15952,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="130" spans="1:40">
+    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -15880,7 +16070,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="131" spans="1:40">
+    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
@@ -15998,7 +16188,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="132" spans="1:40">
+    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
@@ -16116,7 +16306,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="133" spans="1:40">
+    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
@@ -16234,7 +16424,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="134" spans="1:40">
+    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
@@ -16352,7 +16542,7 @@
         <v>-9.1</v>
       </c>
     </row>
-    <row r="135" spans="1:40">
+    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
@@ -16470,7 +16660,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="136" spans="1:40">
+    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
@@ -16588,7 +16778,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="137" spans="1:40">
+    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
@@ -16706,7 +16896,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="138" spans="1:40">
+    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
@@ -16824,7 +17014,7 @@
         <v>-4.7</v>
       </c>
     </row>
-    <row r="139" spans="1:40">
+    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -16942,7 +17132,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="140" spans="1:40">
+    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -17060,7 +17250,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:40">
+    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
@@ -17178,7 +17368,7 @@
         <v>-4.5999999999999996</v>
       </c>
     </row>
-    <row r="142" spans="1:40">
+    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
@@ -17296,7 +17486,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="143" spans="1:40">
+    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
@@ -17414,7 +17604,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="144" spans="1:40">
+    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -17532,7 +17722,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="145" spans="1:40">
+    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -17650,7 +17840,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="146" spans="1:40">
+    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -17768,7 +17958,7 @@
         <v>-6.7</v>
       </c>
     </row>
-    <row r="147" spans="1:40">
+    <row r="147" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -17886,7 +18076,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="148" spans="1:40">
+    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
@@ -18004,7 +18194,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="149" spans="1:40">
+    <row r="149" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
@@ -18122,7 +18312,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="150" spans="1:40">
+    <row r="150" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
@@ -18240,7 +18430,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="151" spans="1:40">
+    <row r="151" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
@@ -18358,7 +18548,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:40">
+    <row r="152" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
@@ -18476,7 +18666,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="153" spans="1:40">
+    <row r="153" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
@@ -18594,7 +18784,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:40">
+    <row r="154" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -18712,7 +18902,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="155" spans="1:40">
+    <row r="155" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
@@ -18830,7 +19020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:40">
+    <row r="156" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
@@ -18948,7 +19138,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="157" spans="1:40">
+    <row r="157" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
@@ -19066,7 +19256,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="158" spans="1:40">
+    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -19184,7 +19374,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="159" spans="1:40">
+    <row r="159" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -19302,7 +19492,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="160" spans="1:40">
+    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
@@ -19420,7 +19610,7 @@
         <v>-2.9</v>
       </c>
     </row>
-    <row r="161" spans="1:40">
+    <row r="161" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -19538,7 +19728,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="162" spans="1:40">
+    <row r="162" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -19656,7 +19846,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="163" spans="1:40">
+    <row r="163" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -19774,7 +19964,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="164" spans="1:40">
+    <row r="164" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -19892,7 +20082,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="165" spans="1:40">
+    <row r="165" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
@@ -20010,7 +20200,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="166" spans="1:40">
+    <row r="166" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
@@ -20128,7 +20318,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="167" spans="1:40">
+    <row r="167" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
@@ -20246,7 +20436,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="168" spans="1:40">
+    <row r="168" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
@@ -20364,7 +20554,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="169" spans="1:40">
+    <row r="169" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
@@ -20482,7 +20672,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:40">
+    <row r="170" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
@@ -20598,7 +20788,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="171" spans="1:40">
+    <row r="171" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
@@ -20718,7 +20908,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="172" spans="1:40">
+    <row r="172" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
@@ -20838,7 +21028,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="173" spans="1:40">
+    <row r="173" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>171</v>
       </c>
@@ -20958,7 +21148,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="174" spans="1:40">
+    <row r="174" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
@@ -21078,7 +21268,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="175" spans="1:40">
+    <row r="175" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
@@ -21198,7 +21388,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="176" spans="1:40">
+    <row r="176" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
@@ -21318,7 +21508,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="177" spans="1:40">
+    <row r="177" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>175</v>
       </c>
@@ -21438,7 +21628,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="178" spans="1:40">
+    <row r="178" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>176</v>
       </c>
@@ -21558,7 +21748,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="179" spans="1:40">
+    <row r="179" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>177</v>
       </c>
@@ -21678,7 +21868,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="180" spans="1:40">
+    <row r="180" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
@@ -21798,7 +21988,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="181" spans="1:40">
+    <row r="181" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
@@ -21918,7 +22108,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="182" spans="1:40">
+    <row r="182" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
@@ -22038,7 +22228,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="183" spans="1:40">
+    <row r="183" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>181</v>
       </c>
@@ -22158,7 +22348,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="184" spans="1:40">
+    <row r="184" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
@@ -22278,7 +22468,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="185" spans="1:40">
+    <row r="185" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
@@ -22398,7 +22588,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="186" spans="1:40">
+    <row r="186" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>184</v>
       </c>
@@ -22518,7 +22708,7 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="187" spans="1:40">
+    <row r="187" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
@@ -22638,7 +22828,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="188" spans="1:40">
+    <row r="188" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
@@ -22758,7 +22948,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="189" spans="1:40">
+    <row r="189" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
@@ -22878,7 +23068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:40">
+    <row r="190" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
@@ -22998,7 +23188,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="191" spans="1:40">
+    <row r="191" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>189</v>
       </c>
@@ -23118,7 +23308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:40">
+    <row r="192" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>190</v>
       </c>
@@ -23238,7 +23428,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="193" spans="1:40">
+    <row r="193" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>191</v>
       </c>
@@ -23358,7 +23548,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:40">
+    <row r="194" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>192</v>
       </c>
@@ -23478,7 +23668,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="195" spans="1:40">
+    <row r="195" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>193</v>
       </c>
@@ -23598,7 +23788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:40">
+    <row r="196" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
@@ -23718,7 +23908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:40">
+    <row r="197" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>195</v>
       </c>
@@ -23838,7 +24028,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="198" spans="1:40">
+    <row r="198" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>196</v>
       </c>
@@ -23958,7 +24148,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="199" spans="1:40">
+    <row r="199" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>197</v>
       </c>
@@ -24078,7 +24268,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="200" spans="1:40">
+    <row r="200" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>198</v>
       </c>
@@ -24198,7 +24388,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="201" spans="1:40">
+    <row r="201" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>199</v>
       </c>
@@ -24318,7 +24508,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="202" spans="1:40">
+    <row r="202" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>200</v>
       </c>
@@ -24438,7 +24628,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="203" spans="1:40">
+    <row r="203" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>201</v>
       </c>
@@ -24558,7 +24748,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="204" spans="1:40">
+    <row r="204" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>202</v>
       </c>
@@ -24678,7 +24868,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="205" spans="1:40">
+    <row r="205" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>203</v>
       </c>
@@ -24798,7 +24988,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="206" spans="1:40">
+    <row r="206" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>204</v>
       </c>
@@ -24912,7 +25102,7 @@
         <v>-8.5</v>
       </c>
     </row>
-    <row r="207" spans="1:40">
+    <row r="207" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>205</v>
       </c>
@@ -25026,7 +25216,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="208" spans="1:40">
+    <row r="208" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>206</v>
       </c>
@@ -25140,7 +25330,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="209" spans="1:40">
+    <row r="209" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>207</v>
       </c>
@@ -25254,7 +25444,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="210" spans="1:40">
+    <row r="210" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>208</v>
       </c>
@@ -25368,7 +25558,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="211" spans="1:40">
+    <row r="211" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>209</v>
       </c>
@@ -25482,7 +25672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:40">
+    <row r="212" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>210</v>
       </c>
@@ -25596,7 +25786,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="213" spans="1:40">
+    <row r="213" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>211</v>
       </c>
@@ -25710,7 +25900,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="214" spans="1:40">
+    <row r="214" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>212</v>
       </c>
@@ -25824,7 +26014,7 @@
         <v>-4.7</v>
       </c>
     </row>
-    <row r="215" spans="1:40">
+    <row r="215" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>213</v>
       </c>
@@ -25938,7 +26128,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="216" spans="1:40">
+    <row r="216" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>214</v>
       </c>
@@ -26052,7 +26242,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="217" spans="1:40">
+    <row r="217" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>215</v>
       </c>
@@ -26166,7 +26356,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="218" spans="1:40">
+    <row r="218" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>216</v>
       </c>
@@ -26280,7 +26470,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="219" spans="1:40">
+    <row r="219" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>217</v>
       </c>
@@ -26394,7 +26584,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="220" spans="1:40">
+    <row r="220" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>218</v>
       </c>
@@ -26508,7 +26698,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="221" spans="1:40">
+    <row r="221" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>219</v>
       </c>
@@ -26622,7 +26812,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="222" spans="1:40">
+    <row r="222" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>220</v>
       </c>
@@ -26736,7 +26926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:40">
+    <row r="223" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>221</v>
       </c>
@@ -26850,7 +27040,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="224" spans="1:40">
+    <row r="224" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
@@ -26964,7 +27154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:40">
+    <row r="225" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>223</v>
       </c>
@@ -27078,7 +27268,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="226" spans="1:40">
+    <row r="226" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>224</v>
       </c>
@@ -27192,7 +27382,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="227" spans="1:40">
+    <row r="227" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>225</v>
       </c>
@@ -27306,7 +27496,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="228" spans="1:40">
+    <row r="228" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>226</v>
       </c>
@@ -27420,7 +27610,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="229" spans="1:40">
+    <row r="229" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>227</v>
       </c>
@@ -27534,7 +27724,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="230" spans="1:40">
+    <row r="230" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>228</v>
       </c>
@@ -27648,7 +27838,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="231" spans="1:40">
+    <row r="231" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>229</v>
       </c>
@@ -27762,7 +27952,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="232" spans="1:40">
+    <row r="232" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>230</v>
       </c>
@@ -27876,7 +28066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:40">
+    <row r="233" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>231</v>
       </c>
@@ -27990,7 +28180,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="234" spans="1:40">
+    <row r="234" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>232</v>
       </c>
@@ -28104,7 +28294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:40">
+    <row r="235" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>233</v>
       </c>
@@ -28218,7 +28408,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="236" spans="1:40">
+    <row r="236" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>234</v>
       </c>
@@ -28332,7 +28522,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="237" spans="1:40">
+    <row r="237" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>235</v>
       </c>
@@ -28446,7 +28636,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="238" spans="1:40">
+    <row r="238" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>236</v>
       </c>
@@ -28560,7 +28750,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="239" spans="1:40">
+    <row r="239" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>237</v>
       </c>
@@ -28674,7 +28864,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="240" spans="1:40">
+    <row r="240" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>238</v>
       </c>
@@ -28788,7 +28978,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="241" spans="1:40">
+    <row r="241" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
@@ -28902,7 +29092,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="242" spans="1:40">
+    <row r="242" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>240</v>
       </c>
@@ -29016,7 +29206,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="243" spans="1:40">
+    <row r="243" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
@@ -29130,7 +29320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:40">
+    <row r="244" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>

</xml_diff>